<commit_message>
Finalize motor controller PCB v0.1
</commit_message>
<xml_diff>
--- a/electrical/TurntableMotorController-BOM.xlsx
+++ b/electrical/TurntableMotorController-BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6832AFDF-8B4B-4F36-BF3B-0650A2A5411B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B19177-A55A-4A18-A7F4-26CCA62C77CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
   <si>
     <t>Ceramic Capacitor</t>
   </si>
@@ -141,9 +141,6 @@
     <t>--</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>Relay</t>
   </si>
   <si>
@@ -153,12 +150,6 @@
     <t>DPDT (2 Form C)</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>D1, D2, D3</t>
-  </si>
-  <si>
     <t>J1, J2, J3, J4</t>
   </si>
   <si>
@@ -171,61 +162,142 @@
     <t>8191</t>
   </si>
   <si>
-    <t>Q1, Q2, Q3</t>
-  </si>
-  <si>
-    <t>R1, R2, R3</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>R7</t>
   </si>
   <si>
-    <t>62Ω</t>
-  </si>
-  <si>
-    <t>200Ω</t>
-  </si>
-  <si>
-    <t>AC05000002000JAC00</t>
-  </si>
-  <si>
-    <t>110Ω</t>
-  </si>
-  <si>
-    <t>SQP500JB-110R</t>
-  </si>
-  <si>
-    <t>ROX5SSJ62R</t>
-  </si>
-  <si>
-    <t>RL1, RL2, RL3</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
-    <t>J10</t>
-  </si>
-  <si>
     <t>KF2510  5-pin</t>
   </si>
   <si>
-    <t>C2, C3, C4</t>
-  </si>
-  <si>
-    <t>1µF; 16V</t>
-  </si>
-  <si>
-    <t>0805YD105KAT2A</t>
-  </si>
-  <si>
     <t>Price estimates are as of 2 Oct. 2022</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>R5, R14</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>RL1</t>
+  </si>
+  <si>
+    <t>22µF; 25v</t>
+  </si>
+  <si>
+    <t>CL21A226MAYNNNE</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C1, C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>0805B471K500CT</t>
+  </si>
+  <si>
+    <t>C5, C6, C7, C8, C9, C10</t>
+  </si>
+  <si>
+    <t>0.47nF; 50v</t>
+  </si>
+  <si>
+    <t>CL21B104KBCNNNC</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4</t>
+  </si>
+  <si>
+    <t>Thumbwheel Potentiometer</t>
+  </si>
+  <si>
+    <t>100 nf; 50v</t>
+  </si>
+  <si>
+    <t>10kΩ; 1/2w</t>
+  </si>
+  <si>
+    <t>3352W-1-103LF</t>
+  </si>
+  <si>
+    <t>69kΩ</t>
+  </si>
+  <si>
+    <t>RN73H1JTTD6902D100</t>
+  </si>
+  <si>
+    <t>R6, R10</t>
+  </si>
+  <si>
+    <t>26.7kΩ</t>
+  </si>
+  <si>
+    <t>RC0603FR-0726K7L</t>
+  </si>
+  <si>
+    <t>R8, R9</t>
+  </si>
+  <si>
+    <t>47kΩ</t>
+  </si>
+  <si>
+    <t>RG1608P-473-B-T5</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>104kΩ</t>
+  </si>
+  <si>
+    <t>RN73H1JTTD1043B50</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>94kΩ</t>
+  </si>
+  <si>
+    <t>RT0603BRD0794K2L</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>Variable Voltage Regulator</t>
+  </si>
+  <si>
+    <t>12v; 5a</t>
+  </si>
+  <si>
+    <t>AZ1084CS2-ADJTRE1</t>
+  </si>
+  <si>
+    <t>U3, U4, U5, U6, U7, U8</t>
+  </si>
+  <si>
+    <t>Demultiplexer 1:2</t>
+  </si>
+  <si>
+    <t>ISL43210IHZ-T7A</t>
+  </si>
+  <si>
+    <t>DG9431EDV-T1-GE3</t>
   </si>
 </sst>
 </file>
@@ -871,8 +943,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
@@ -1186,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1312,7 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1259,130 +1331,138 @@
         <v>23</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2" s="15">
-        <v>0.65</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>23</v>
+      <c r="G3" s="8">
+        <v>805</v>
       </c>
       <c r="H3" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I3" s="6">
-        <v>0.72</v>
+        <v>0.25</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="5">
-        <v>3</v>
-      </c>
       <c r="I4" s="9">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="7"/>
       <c r="F5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="H5" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I5" s="6">
-        <v>2.08</v>
+        <v>0.6</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="D6" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="H6" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6" s="6">
-        <v>3</v>
+        <v>0.22</v>
       </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="4"/>
+      <c r="C7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1390,27 +1470,27 @@
         <v>17</v>
       </c>
       <c r="H7" s="5">
-        <v>3</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0.33</v>
+        <v>2</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.78</v>
       </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="C8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1420,254 +1500,416 @@
       <c r="H8" s="5">
         <v>1</v>
       </c>
-      <c r="I8" s="6">
-        <v>0.16</v>
+      <c r="I8" s="9">
+        <v>0.1</v>
       </c>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
-        <v>52</v>
+        <v>72</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="H9" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="9">
-        <v>0.93</v>
+        <v>0.76</v>
       </c>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="H10" s="5">
         <v>1</v>
       </c>
-      <c r="I10" s="6">
-        <v>0.64</v>
+      <c r="I10" s="9">
+        <v>0.53</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C11" s="8" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="H11" s="5">
         <v>1</v>
       </c>
       <c r="I11" s="9">
-        <v>0.74</v>
+        <v>0.34</v>
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5" t="s">
-        <v>38</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="H12" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I12" s="6">
-        <v>3.93</v>
+        <v>0.16</v>
       </c>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I13" s="6">
-        <v>4.7</v>
+        <v>17.52</v>
       </c>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D14" s="5" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="G14" s="4"/>
       <c r="H14" s="5">
         <v>1</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9">
+        <v>0.11</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="5">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="5">
+        <v>4</v>
+      </c>
+      <c r="I18" s="9">
+        <v>10</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6">
+        <f>3.93/3</f>
+        <v>1.31</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="5">
+        <v>4</v>
+      </c>
+      <c r="I20" s="6">
+        <v>2.08</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12">
-        <f>SUM(H2:H14)</f>
-        <v>26</v>
-      </c>
-      <c r="I15" s="13">
-        <f>SUM(I2:I14)</f>
-        <v>18.21</v>
-      </c>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="12">
+        <f>SUM(H2:H21)</f>
+        <v>40</v>
+      </c>
+      <c r="I22" s="13">
+        <f>SUM(I2:I21)</f>
+        <v>42.58</v>
+      </c>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1677,6 +1919,11 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
@@ -1687,31 +1934,36 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+    </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-    </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
@@ -1722,10 +1974,10 @@
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
@@ -1737,11 +1989,6 @@
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-    </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
@@ -1752,11 +1999,6 @@
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-    </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
@@ -1796,6 +2038,41 @@
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Merge StrobeController board into MotorController
</commit_message>
<xml_diff>
--- a/electrical/TurntableMotorController-BOM.xlsx
+++ b/electrical/TurntableMotorController-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B19177-A55A-4A18-A7F4-26CCA62C77CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6B4D6F-E89A-4F66-B75E-ECECBD60A0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
   <si>
     <t>Ceramic Capacitor</t>
   </si>
@@ -183,9 +183,6 @@
     <t>J5</t>
   </si>
   <si>
-    <t>R5, R14</t>
-  </si>
-  <si>
     <t>R13</t>
   </si>
   <si>
@@ -298,6 +295,27 @@
   </si>
   <si>
     <t>DG9431EDV-T1-GE3</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>male header 2 pins (1 row)</t>
+  </si>
+  <si>
+    <t>KF2510  2-pin</t>
+  </si>
+  <si>
+    <t>R5, R14, R15</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Screw terminal (2 pins)</t>
+  </si>
+  <si>
+    <t>ED10563-ND</t>
   </si>
 </sst>
 </file>
@@ -943,8 +961,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J24" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
@@ -1258,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,7 +1330,7 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1339,23 +1357,23 @@
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="8">
-        <v>805</v>
+      <c r="G3" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
@@ -1367,16 +1385,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
@@ -1395,16 +1413,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="5" t="s">
@@ -1423,7 +1441,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>19</v>
@@ -1442,25 +1460,25 @@
         <v>17</v>
       </c>
       <c r="H6" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6" s="6">
-        <v>0.22</v>
+        <v>0.33</v>
       </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
@@ -1485,10 +1503,10 @@
         <v>19</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
@@ -1507,16 +1525,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
@@ -1535,16 +1553,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
@@ -1563,16 +1581,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
@@ -1591,7 +1609,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>19</v>
@@ -1619,19 +1637,19 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>12</v>
@@ -1647,16 +1665,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
@@ -1753,16 +1771,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="C18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
@@ -1779,7 +1797,7 @@
     </row>
     <row r="19" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>36</v>
@@ -1855,49 +1873,87 @@
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0.41</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="12">
-        <f>SUM(H2:H21)</f>
-        <v>40</v>
-      </c>
-      <c r="I22" s="13">
-        <f>SUM(I2:I21)</f>
-        <v>42.58</v>
-      </c>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="12">
+        <f>SUM(H2:H22)</f>
+        <v>42</v>
+      </c>
+      <c r="I24" s="13">
+        <f>SUM(I2:I22)</f>
+        <v>42.69</v>
+      </c>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -1954,61 +2010,61 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+    </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+    </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-    </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
@@ -2073,6 +2129,16 @@
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>